<commit_message>
1. Minor Correction 2. requirement.txt file
</commit_message>
<xml_diff>
--- a/data/testfile.xlsx
+++ b/data/testfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mandar.potdar\PycharmProjects\PlaywrightPython\PlaywrightPython\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mandar.potdar\PycharmProjects\PlaywrightPython\PlaywrightPython\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEDAD4F-83A3-4235-8600-A49A7E091BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE289A9-7360-4C26-A145-E361F275F7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6750" yWindow="4515" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
@@ -397,6 +397,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>